<commit_message>
AJUSTES E IMPLEMENTAÇÃO ETIQUETA REQUISICAO
</commit_message>
<xml_diff>
--- a/SIG/Producao/Producao/Modelos/PROGRAMACAO_PROGRAMACAO_MODELO.xlsx
+++ b/SIG/Producao/Producao/Modelos/PROGRAMACAO_PROGRAMACAO_MODELO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Repos\wognascimento\SIG\SIG\Producao\Producao\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713939FF-1652-4D0B-ACE8-3B00B91BB350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF75548-4D26-414F-9331-0E05C914A424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{D9A668C6-916A-46D2-B14A-67ECE735CF5F}"/>
   </bookViews>
@@ -232,17 +232,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,7 +577,7 @@
   <cols>
     <col min="1" max="1" width="1.140625" customWidth="1"/>
     <col min="2" max="2" width="4.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
@@ -619,20 +619,20 @@
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="L3" s="10"/>
-      <c r="M3" s="5"/>
+      <c r="M3" s="7"/>
       <c r="N3" s="1">
         <f>COUNTIF(N9:N1048576,"FILA/M.O")</f>
         <v>0</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="10"/>
-      <c r="Q3" s="5"/>
+      <c r="Q3" s="7"/>
       <c r="R3" s="1">
         <f>COUNTIF(N9:N1048576,"INDEFINIDO")</f>
         <v>0</v>
@@ -641,27 +641,27 @@
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="4" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="L4" s="10"/>
-      <c r="M4" s="5"/>
+      <c r="M4" s="7"/>
       <c r="N4" s="1">
         <f>COUNTIF(N9:N1048576,"EM ANDAMENTO")</f>
         <v>0</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="P4" s="10"/>
-      <c r="Q4" s="5"/>
+      <c r="Q4" s="7"/>
       <c r="R4" s="1">
         <f>COUNTIF(N9:N1048576,"PROJETOS")</f>
         <v>0</v>
@@ -670,27 +670,27 @@
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="4" t="s">
+      <c r="G5" s="7"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="L5" s="10"/>
-      <c r="M5" s="5"/>
+      <c r="M5" s="7"/>
       <c r="N5" s="1">
         <f>COUNTIF(N9:N1048576,"EMBALAGEM/EXPEDIÇÃO")</f>
         <v>0</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="P5" s="10"/>
-      <c r="Q5" s="5"/>
+      <c r="Q5" s="7"/>
       <c r="R5" s="1">
         <f>COUNTIF(N9:N1048576,"FALTA MATERIAL INTERNO / TRANSF")</f>
         <v>0</v>
@@ -699,20 +699,20 @@
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="L6" s="10"/>
-      <c r="M6" s="5"/>
+      <c r="M6" s="7"/>
       <c r="N6" s="1">
         <f>COUNTIF(N9:N1048576,"ESPAÇO FÍSICO")</f>
         <v>0</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="P6" s="10"/>
-      <c r="Q6" s="5"/>
+      <c r="Q6" s="7"/>
       <c r="R6" s="1">
         <f>COUNTIF(N9:N1048576,"FALTA MATERIAL EXTERNO / COMPRAS")</f>
         <v>0</v>
@@ -765,11 +765,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B1:T1"/>
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="P8:Q8"/>
     <mergeCell ref="N8:O8"/>
@@ -782,11 +777,16 @@
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="K6:M6"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B1:T1"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="90" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="89" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;RPágina &amp;P de &amp;N</oddFooter>
+    <oddFooter>&amp;LProgramação impressa em  &amp;D&amp;RPágina &amp;P de &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>